<commit_message>
Update (not working version)
</commit_message>
<xml_diff>
--- a/helper_files/Book1.xlsx
+++ b/helper_files/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\surfdrive\R\ANOVA_power_simulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\surfdrive\R\ANOVA_power_simulation\helper_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDDE3A8-3402-4607-AF7A-A4A7D9D9F5AB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D40A98-EFCA-4264-9B5D-7D6D223316A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6906" activeTab="1" xr2:uid="{13DA85A8-B127-4206-A4A0-14E158E8E29A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6906" xr2:uid="{13DA85A8-B127-4206-A4A0-14E158E8E29A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="71">
   <si>
     <t>2wx3b</t>
   </si>
@@ -224,6 +224,21 @@
   </si>
   <si>
     <t>repeat</t>
+  </si>
+  <si>
+    <t>2bx3wx2w</t>
+  </si>
+  <si>
+    <t>a1b3c1</t>
+  </si>
+  <si>
+    <t>a1b3c2</t>
+  </si>
+  <si>
+    <t>a2b3c1</t>
+  </si>
+  <si>
+    <t>a2b3c2</t>
   </si>
 </sst>
 </file>
@@ -581,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A02B21-7962-4D84-B356-5B738081ABF0}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1130,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1183,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1236,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="I19" t="s">
         <v>10</v>
       </c>
@@ -1268,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="I20" t="s">
         <v>11</v>
       </c>
@@ -1300,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="I21" t="s">
         <v>13</v>
       </c>
@@ -1332,12 +1347,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="L23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>15</v>
       </c>
@@ -1362,28 +1380,64 @@
       <c r="I24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="L24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" t="s">
+        <v>18</v>
+      </c>
+      <c r="O24" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>68</v>
+      </c>
+      <c r="R24" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" t="s">
+        <v>20</v>
+      </c>
+      <c r="T24" t="s">
+        <v>21</v>
+      </c>
+      <c r="U24" t="s">
+        <v>22</v>
+      </c>
+      <c r="V24" t="s">
+        <v>69</v>
+      </c>
+      <c r="W24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1</v>
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
       </c>
-      <c r="F25" s="1">
-        <v>0</v>
-      </c>
-      <c r="G25" s="1">
-        <v>0</v>
+      <c r="F25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="H25" s="1">
         <v>0</v>
@@ -1391,13 +1445,52 @@
       <c r="I25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0</v>
+      </c>
+      <c r="T25" s="1">
+        <v>0</v>
+      </c>
+      <c r="U25" s="1">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0</v>
+      </c>
+      <c r="W25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="1">
-        <v>0</v>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -1405,14 +1498,14 @@
       <c r="D26" s="1">
         <v>0</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -1420,13 +1513,52 @@
       <c r="I26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1">
+        <v>0</v>
+      </c>
+      <c r="T26" s="1">
+        <v>0</v>
+      </c>
+      <c r="U26" s="1">
+        <v>0</v>
+      </c>
+      <c r="V26" s="1">
+        <v>0</v>
+      </c>
+      <c r="W26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>1</v>
+      <c r="B27" s="1">
+        <v>0</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -1434,8 +1566,8 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="E27" s="1">
-        <v>0</v>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1443,22 +1575,65 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1">
+        <v>1</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" s="1">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1">
+        <v>0</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0</v>
+      </c>
+      <c r="U27" s="1">
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
+        <v>0</v>
+      </c>
+      <c r="W27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1"/>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E28" s="1">
         <v>1</v>
       </c>
@@ -1468,22 +1643,61 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="1">
-        <v>0</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="H28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>0</v>
+      </c>
+      <c r="S28" s="1">
+        <v>0</v>
+      </c>
+      <c r="T28" s="1">
+        <v>0</v>
+      </c>
+      <c r="U28" s="1">
+        <v>0</v>
+      </c>
+      <c r="V28" s="1">
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="1">
-        <v>0</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0</v>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -1494,21 +1708,64 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P29" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1">
+        <v>0</v>
+      </c>
+      <c r="T29" s="1">
+        <v>0</v>
+      </c>
+      <c r="U29" s="1">
+        <v>0</v>
+      </c>
+      <c r="V29" s="1">
+        <v>0</v>
+      </c>
+      <c r="W29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="1">
-        <v>0</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
+      <c r="B30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -1516,16 +1773,59 @@
       <c r="E30" s="1">
         <v>0</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="G30" s="1">
         <v>1</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>1</v>
+      </c>
+      <c r="R30" s="1">
+        <v>0</v>
+      </c>
+      <c r="S30" s="1">
+        <v>0</v>
+      </c>
+      <c r="T30" s="1">
+        <v>0</v>
+      </c>
+      <c r="U30" s="1">
+        <v>0</v>
+      </c>
+      <c r="V30" s="1">
+        <v>0</v>
+      </c>
+      <c r="W30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1535,22 +1835,65 @@
       <c r="C31" s="1">
         <v>0</v>
       </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
       <c r="H31" s="1">
         <v>1</v>
       </c>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="I31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+      <c r="R31" s="1">
+        <v>1</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1560,18 +1903,225 @@
       <c r="C32" s="1">
         <v>0</v>
       </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="I32" s="1">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1">
+        <v>0</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S32" s="1">
+        <v>1</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="11:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="K33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>0</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="11:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="K34" t="s">
+        <v>22</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>0</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U34" s="1">
+        <v>1</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="11:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="K35" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0</v>
+      </c>
+      <c r="N35" s="1">
+        <v>0</v>
+      </c>
+      <c r="O35" s="1">
+        <v>0</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>0</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V35" s="1">
+        <v>1</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="11:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>0</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W36" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1585,9 +2135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBF7C44-A84A-4A13-9358-E982646D0AF7}">
   <dimension ref="A1:XFD52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>

</xml_diff>